<commit_message>
Atualização dos dados 22.12.2025
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0114DE9-7A2D-45B4-AE42-425B9BCF2CDA}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A4861D-65E5-4A1F-A7AC-24D107D8B84A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,177 +688,201 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <f>3*41309</f>
+        <v>123927</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6*F6</f>
+        <v>185890.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1459</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4.2256944444444444E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6657</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2">
+        <v>46012</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <f>3*26209</f>
+        <v>78627</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7*F7</f>
+        <v>117940.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>293</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1311</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3.4004629629629628E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6695</v>
+      </c>
       <c r="J7" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2">
+        <v>46013</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 22.11.2025 08:59
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f>C2*F2</f>
+        <f t="shared" ref="D2:D7" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -577,7 +577,7 @@
         <v>65649</v>
       </c>
       <c r="D3" s="1">
-        <f>C3*F3</f>
+        <f t="shared" si="0"/>
         <v>131298</v>
       </c>
       <c r="E3" s="1">
@@ -616,7 +616,7 @@
         <v>58596</v>
       </c>
       <c r="D4" s="1">
-        <f>C4*F4</f>
+        <f t="shared" si="0"/>
         <v>87894</v>
       </c>
       <c r="E4" s="1">
@@ -656,7 +656,7 @@
         <v>145401</v>
       </c>
       <c r="D5" s="1">
-        <f>C5*F5</f>
+        <f t="shared" si="0"/>
         <v>290802</v>
       </c>
       <c r="E5" s="1">
@@ -696,7 +696,7 @@
         <v>123927</v>
       </c>
       <c r="D6" s="1">
-        <f>C6*F6</f>
+        <f t="shared" si="0"/>
         <v>185890.5</v>
       </c>
       <c r="E6" s="1">
@@ -736,7 +736,7 @@
         <v>78627</v>
       </c>
       <c r="D7" s="1">
-        <f>C7*F7</f>
+        <f t="shared" si="0"/>
         <v>117940.5</v>
       </c>
       <c r="E7" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 22.12.2025 18:20
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A4861D-65E5-4A1F-A7AC-24D107D8B84A}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351D3F0B-95FE-4D19-B3B7-D7D79AF7541F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D7" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D8" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -666,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="1">
-        <v>262</v>
+        <v>1262</v>
       </c>
       <c r="H5" s="4">
         <v>3.9548611111111111E-2</v>
@@ -768,7 +768,41 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="B8" s="1">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <f>3*38835</f>
+        <v>116505</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>174757.5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>277</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1411</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4.2418981481481481E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>6700</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="2">
+        <v>46013</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 23.12.2025 09:04
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351D3F0B-95FE-4D19-B3B7-D7D79AF7541F}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A91731-7647-470E-872E-D5B721D49177}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D8" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D9" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -808,7 +808,40 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>59291</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>118582</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1134</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4.221064814814815E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6783</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>46014</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 23.12.2025 15:57
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A91731-7647-470E-872E-D5B721D49177}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A38A880-C0F1-4361-98C0-A4D72740FBBD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D9" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D10" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -847,7 +847,41 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <f>3*29054</f>
+        <v>87162</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>174324</v>
+      </c>
+      <c r="E10" s="1">
+        <v>389</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1366</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3.439814814814815E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>6800</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="2">
+        <v>46014</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 23.12.2025 23:42
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A38A880-C0F1-4361-98C0-A4D72740FBBD}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440BFAB0-6AC2-4F43-B7E5-1D25A468F4A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D10" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D11" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -887,7 +887,41 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="B11" s="1">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1">
+        <f>3*41548</f>
+        <v>124644</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>249288</v>
+      </c>
+      <c r="E11" s="1">
+        <v>484</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1697</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4.4398148148148145E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>6887</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2">
+        <v>46014</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 24.12.2025 09:02
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440BFAB0-6AC2-4F43-B7E5-1D25A468F4A6}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9373861-1D6D-4F83-B42F-26E5E7297E7C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D11" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D12" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -927,7 +927,40 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="B12" s="1">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>41007</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>61510.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1083</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3.847222222222222E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>6900</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>46015</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 26.12.2025 10:6
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9373861-1D6D-4F83-B42F-26E5E7297E7C}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6077BAA5-FDC2-4285-A979-144E7BF86B13}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D12" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D13" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -966,7 +966,40 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="B13" s="1">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1">
+        <v>104495</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>156742.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1750</v>
+      </c>
+      <c r="H13" s="4">
+        <v>5.6388888888888891E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>6980</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="2">
+        <v>46017</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">

</xml_diff>

<commit_message>
Atualização dos dados: 27.12.2025 09:38
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6077BAA5-FDC2-4285-A979-144E7BF86B13}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{455E1399-7364-4AC2-A12B-C961E3EC7CB6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11976C8-4D46-4F6C-B729-AA642E1E63CD}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D13" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D14" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -1005,205 +1005,79 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="B14" s="1">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1">
+        <v>69725</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>104587.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>106</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1588</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5.0231481481481481E-2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>7000</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="2">
+        <v>46018</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização dos dados: 28.12.2025 20:04
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a51e1d9e0f733e61/Documentos/Dungeon Slasher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{455E1399-7364-4AC2-A12B-C961E3EC7CB6}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{741D0274-BF39-48D9-8A4B-BCC2FE5FA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E283A1B2-04CA-455E-A866-AE960F0E2559}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E91225A-01F6-4339-B529-34DD74C38487}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>71835</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D14" si="0">C2*F2</f>
+        <f t="shared" ref="D2:D15" si="0">C2*F2</f>
         <v>143670</v>
       </c>
       <c r="E2" s="1">
@@ -1041,7 +1041,44 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="5"/>
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
+        <f>3*23301</f>
+        <v>69903</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>104854.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>313</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1410</v>
+      </c>
+      <c r="H15" s="4">
+        <v>3.7280092592592594E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>7072</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="2">
+        <v>46020</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J16" s="5"/>

</xml_diff>